<commit_message>
Inclusão do nome dos municípios ao mapa
</commit_message>
<xml_diff>
--- a/USER_PE.xlsx
+++ b/USER_PE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://brennandcimentos-my.sharepoint.com/personal/humberto_araujo_ext_cimentonacional_com_br/Documents/ATIVIDADES/2024-07-01_AUTOMACAO COMERCIAL/ENTRADA/Automacao-de-mapas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\bkp_humberto\PROJETOS\202-08-10_AUTOMACAO\Automacao-de-mapas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{4FDCCE05-4DA3-460D-B982-FF4483FA28C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C77BFC09-E292-4BC9-8F8B-7E786ECF24AF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC80ABC4-8C2C-4EB6-A2F6-7FE69F5DBF5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="300" windowWidth="21840" windowHeight="13020" xr2:uid="{332BFF9F-C31F-4FFC-BF04-3847F4813181}"/>
+    <workbookView xWindow="-21720" yWindow="2505" windowWidth="21840" windowHeight="13020" xr2:uid="{332BFF9F-C31F-4FFC-BF04-3847F4813181}"/>
   </bookViews>
   <sheets>
     <sheet name="PE_DISTRI_CONSULT" sheetId="2" r:id="rId1"/>
@@ -52,9 +52,6 @@
     <t>CD_MUN</t>
   </si>
   <si>
-    <t>NM_MUNICIP</t>
-  </si>
-  <si>
     <t>CONSULTOR</t>
   </si>
   <si>
@@ -650,6 +647,9 @@
   </si>
   <si>
     <t>XEXÉU</t>
+  </si>
+  <si>
+    <t>NM_MUN</t>
   </si>
 </sst>
 </file>
@@ -732,7 +732,7 @@
   <autoFilter ref="A1:D186" xr:uid="{49AA0CE4-403F-4569-8204-05B9A44448C3}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{6AF3C535-0F2D-4928-8BD2-11487A3A37CD}" uniqueName="1" name="CD_MUN" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{8BEEC77F-6412-4B71-9D95-503CF64D6DAA}" uniqueName="2" name="NM_MUNICIP" queryTableFieldId="2" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{8BEEC77F-6412-4B71-9D95-503CF64D6DAA}" uniqueName="2" name="NM_MUN" queryTableFieldId="2" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{5398B68F-69D2-4879-AE0C-2636E9477EFF}" uniqueName="3" name="CONSULTOR" queryTableFieldId="3" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{BE4B7AE1-4662-47CF-BE2D-BEA63C788492}" uniqueName="4" name="DISTRIBUIDOR" queryTableFieldId="4" dataDxfId="0"/>
   </tableColumns>
@@ -1059,7 +1059,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8C9855B-D194-4D29-B8FD-917C39BFDA39}">
   <dimension ref="A1:D186"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1074,13 +1076,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1088,13 +1090,13 @@
         <v>2600054</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1102,13 +1104,13 @@
         <v>2600104</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1116,13 +1118,13 @@
         <v>2600203</v>
       </c>
       <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1130,13 +1132,13 @@
         <v>2600302</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1144,13 +1146,13 @@
         <v>2600401</v>
       </c>
       <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1158,13 +1160,13 @@
         <v>2600500</v>
       </c>
       <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
         <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1172,13 +1174,13 @@
         <v>2600609</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1186,13 +1188,13 @@
         <v>2600708</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -1200,13 +1202,13 @@
         <v>2600807</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -1214,13 +1216,13 @@
         <v>2600906</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1228,13 +1230,13 @@
         <v>2601003</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -1242,13 +1244,13 @@
         <v>2601052</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -1256,13 +1258,13 @@
         <v>2601102</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -1270,13 +1272,13 @@
         <v>2601201</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -1284,13 +1286,13 @@
         <v>2601300</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -1298,13 +1300,13 @@
         <v>2601409</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -1312,13 +1314,13 @@
         <v>2601508</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -1326,13 +1328,13 @@
         <v>2601607</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -1340,13 +1342,13 @@
         <v>2601706</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -1354,13 +1356,13 @@
         <v>2601805</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D21" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -1368,13 +1370,13 @@
         <v>2601904</v>
       </c>
       <c r="B22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -1382,13 +1384,13 @@
         <v>2602001</v>
       </c>
       <c r="B23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -1396,13 +1398,13 @@
         <v>2602100</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -1410,13 +1412,13 @@
         <v>2602209</v>
       </c>
       <c r="B25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -1424,13 +1426,13 @@
         <v>2602308</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -1438,13 +1440,13 @@
         <v>2602407</v>
       </c>
       <c r="B27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -1452,13 +1454,13 @@
         <v>2602506</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -1466,13 +1468,13 @@
         <v>2602605</v>
       </c>
       <c r="B29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -1480,13 +1482,13 @@
         <v>2602704</v>
       </c>
       <c r="B30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C30" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -1494,13 +1496,13 @@
         <v>2602803</v>
       </c>
       <c r="B31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -1508,13 +1510,13 @@
         <v>2602902</v>
       </c>
       <c r="B32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D32" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -1522,13 +1524,13 @@
         <v>2603009</v>
       </c>
       <c r="B33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D33" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -1536,13 +1538,13 @@
         <v>2603108</v>
       </c>
       <c r="B34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D34" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1550,13 +1552,13 @@
         <v>2603207</v>
       </c>
       <c r="B35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D35" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1564,13 +1566,13 @@
         <v>2603306</v>
       </c>
       <c r="B36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D36" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -1578,13 +1580,13 @@
         <v>2603405</v>
       </c>
       <c r="B37" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -1592,13 +1594,13 @@
         <v>2603454</v>
       </c>
       <c r="B38" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" t="s">
         <v>48</v>
-      </c>
-      <c r="C38" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -1606,13 +1608,13 @@
         <v>2603504</v>
       </c>
       <c r="B39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C39" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D39" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -1620,13 +1622,13 @@
         <v>2603603</v>
       </c>
       <c r="B40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C40" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D40" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -1634,13 +1636,13 @@
         <v>2603702</v>
       </c>
       <c r="B41" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C41" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D41" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -1648,13 +1650,13 @@
         <v>2603801</v>
       </c>
       <c r="B42" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C42" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D42" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -1662,13 +1664,13 @@
         <v>2603900</v>
       </c>
       <c r="B43" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C43" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D43" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -1676,13 +1678,13 @@
         <v>2603926</v>
       </c>
       <c r="B44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C44" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D44" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -1690,13 +1692,13 @@
         <v>2604007</v>
       </c>
       <c r="B45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C45" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D45" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -1704,13 +1706,13 @@
         <v>2604106</v>
       </c>
       <c r="B46" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C46" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D46" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -1718,13 +1720,13 @@
         <v>2604155</v>
       </c>
       <c r="B47" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C47" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D47" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -1732,13 +1734,13 @@
         <v>2604205</v>
       </c>
       <c r="B48" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C48" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D48" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -1746,13 +1748,13 @@
         <v>2604304</v>
       </c>
       <c r="B49" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C49" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D49" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -1760,13 +1762,13 @@
         <v>2604403</v>
       </c>
       <c r="B50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C50" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D50" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -1774,13 +1776,13 @@
         <v>2604502</v>
       </c>
       <c r="B51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C51" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D51" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -1788,13 +1790,13 @@
         <v>2604601</v>
       </c>
       <c r="B52" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C52" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D52" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -1802,13 +1804,13 @@
         <v>2604700</v>
       </c>
       <c r="B53" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C53" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D53" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -1816,13 +1818,13 @@
         <v>2604809</v>
       </c>
       <c r="B54" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C54" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D54" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -1830,13 +1832,13 @@
         <v>2604908</v>
       </c>
       <c r="B55" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C55" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D55" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -1844,13 +1846,13 @@
         <v>2605004</v>
       </c>
       <c r="B56" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C56" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D56" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -1858,13 +1860,13 @@
         <v>2605103</v>
       </c>
       <c r="B57" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C57" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D57" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -1872,13 +1874,13 @@
         <v>2605152</v>
       </c>
       <c r="B58" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C58" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D58" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -1886,13 +1888,13 @@
         <v>2605202</v>
       </c>
       <c r="B59" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C59" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D59" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -1900,13 +1902,13 @@
         <v>2605301</v>
       </c>
       <c r="B60" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C60" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D60" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -1914,13 +1916,13 @@
         <v>2605400</v>
       </c>
       <c r="B61" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C61" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D61" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -1928,13 +1930,13 @@
         <v>2605459</v>
       </c>
       <c r="B62" t="s">
+        <v>72</v>
+      </c>
+      <c r="C62" t="s">
         <v>73</v>
       </c>
-      <c r="C62" t="s">
-        <v>74</v>
-      </c>
       <c r="D62" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -1942,13 +1944,13 @@
         <v>2605509</v>
       </c>
       <c r="B63" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C63" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D63" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
@@ -1956,13 +1958,13 @@
         <v>2605608</v>
       </c>
       <c r="B64" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C64" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D64" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -1970,13 +1972,13 @@
         <v>2605707</v>
       </c>
       <c r="B65" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C65" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D65" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -1984,13 +1986,13 @@
         <v>2605806</v>
       </c>
       <c r="B66" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C66" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D66" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
@@ -1998,13 +2000,13 @@
         <v>2605905</v>
       </c>
       <c r="B67" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C67" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D67" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
@@ -2012,13 +2014,13 @@
         <v>2606002</v>
       </c>
       <c r="B68" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C68" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D68" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
@@ -2026,13 +2028,13 @@
         <v>2606101</v>
       </c>
       <c r="B69" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C69" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D69" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -2040,13 +2042,13 @@
         <v>2606200</v>
       </c>
       <c r="B70" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C70" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D70" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
@@ -2054,13 +2056,13 @@
         <v>2606309</v>
       </c>
       <c r="B71" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C71" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D71" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
@@ -2068,13 +2070,13 @@
         <v>2606408</v>
       </c>
       <c r="B72" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C72" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D72" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
@@ -2082,13 +2084,13 @@
         <v>2606507</v>
       </c>
       <c r="B73" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C73" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D73" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
@@ -2096,13 +2098,13 @@
         <v>2606606</v>
       </c>
       <c r="B74" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C74" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D74" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
@@ -2110,13 +2112,13 @@
         <v>2606705</v>
       </c>
       <c r="B75" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C75" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D75" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
@@ -2124,13 +2126,13 @@
         <v>2606804</v>
       </c>
       <c r="B76" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C76" t="s">
+        <v>4</v>
+      </c>
+      <c r="D76" t="s">
         <v>5</v>
-      </c>
-      <c r="D76" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
@@ -2138,13 +2140,13 @@
         <v>2606903</v>
       </c>
       <c r="B77" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C77" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D77" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
@@ -2152,13 +2154,13 @@
         <v>2607604</v>
       </c>
       <c r="B78" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C78" t="s">
+        <v>4</v>
+      </c>
+      <c r="D78" t="s">
         <v>5</v>
-      </c>
-      <c r="D78" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
@@ -2166,13 +2168,13 @@
         <v>2607000</v>
       </c>
       <c r="B79" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C79" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D79" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
@@ -2180,13 +2182,13 @@
         <v>2607109</v>
       </c>
       <c r="B80" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C80" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D80" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
@@ -2194,13 +2196,13 @@
         <v>2607208</v>
       </c>
       <c r="B81" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C81" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D81" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
@@ -2208,13 +2210,13 @@
         <v>2607307</v>
       </c>
       <c r="B82" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C82" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D82" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
@@ -2222,13 +2224,13 @@
         <v>2607406</v>
       </c>
       <c r="B83" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C83" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D83" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
@@ -2236,13 +2238,13 @@
         <v>2607505</v>
       </c>
       <c r="B84" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C84" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D84" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
@@ -2250,13 +2252,13 @@
         <v>2607653</v>
       </c>
       <c r="B85" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C85" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D85" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
@@ -2264,13 +2266,13 @@
         <v>2607703</v>
       </c>
       <c r="B86" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C86" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D86" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
@@ -2278,13 +2280,13 @@
         <v>2607752</v>
       </c>
       <c r="B87" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C87" t="s">
+        <v>4</v>
+      </c>
+      <c r="D87" t="s">
         <v>5</v>
-      </c>
-      <c r="D87" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
@@ -2292,13 +2294,13 @@
         <v>2607802</v>
       </c>
       <c r="B88" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C88" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D88" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
@@ -2306,13 +2308,13 @@
         <v>2607901</v>
       </c>
       <c r="B89" t="s">
+        <v>100</v>
+      </c>
+      <c r="C89" t="s">
+        <v>14</v>
+      </c>
+      <c r="D89" t="s">
         <v>101</v>
-      </c>
-      <c r="C89" t="s">
-        <v>15</v>
-      </c>
-      <c r="D89" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
@@ -2320,13 +2322,13 @@
         <v>2607950</v>
       </c>
       <c r="B90" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C90" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D90" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
@@ -2334,13 +2336,13 @@
         <v>2608008</v>
       </c>
       <c r="B91" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C91" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D91" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
@@ -2348,13 +2350,13 @@
         <v>2608057</v>
       </c>
       <c r="B92" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C92" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D92" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
@@ -2362,13 +2364,13 @@
         <v>2608107</v>
       </c>
       <c r="B93" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C93" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D93" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
@@ -2376,13 +2378,13 @@
         <v>2608206</v>
       </c>
       <c r="B94" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C94" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D94" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
@@ -2390,13 +2392,13 @@
         <v>2608255</v>
       </c>
       <c r="B95" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C95" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D95" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
@@ -2404,13 +2406,13 @@
         <v>2608305</v>
       </c>
       <c r="B96" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C96" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D96" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
@@ -2418,13 +2420,13 @@
         <v>2608404</v>
       </c>
       <c r="B97" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C97" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D97" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
@@ -2432,13 +2434,13 @@
         <v>2608503</v>
       </c>
       <c r="B98" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C98" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D98" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
@@ -2446,13 +2448,13 @@
         <v>2608453</v>
       </c>
       <c r="B99" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C99" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D99" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
@@ -2460,13 +2462,13 @@
         <v>2608602</v>
       </c>
       <c r="B100" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C100" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D100" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
@@ -2474,13 +2476,13 @@
         <v>2608701</v>
       </c>
       <c r="B101" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C101" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D101" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
@@ -2488,13 +2490,13 @@
         <v>2608750</v>
       </c>
       <c r="B102" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C102" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D102" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
@@ -2502,13 +2504,13 @@
         <v>2608800</v>
       </c>
       <c r="B103" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C103" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D103" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
@@ -2516,13 +2518,13 @@
         <v>2608909</v>
       </c>
       <c r="B104" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C104" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D104" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
@@ -2530,13 +2532,13 @@
         <v>2609006</v>
       </c>
       <c r="B105" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C105" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D105" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
@@ -2544,13 +2546,13 @@
         <v>2609105</v>
       </c>
       <c r="B106" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C106" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D106" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
@@ -2558,13 +2560,13 @@
         <v>2609154</v>
       </c>
       <c r="B107" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C107" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D107" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
@@ -2572,13 +2574,13 @@
         <v>2609204</v>
       </c>
       <c r="B108" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C108" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D108" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
@@ -2586,13 +2588,13 @@
         <v>2609303</v>
       </c>
       <c r="B109" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C109" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D109" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
@@ -2600,13 +2602,13 @@
         <v>2614303</v>
       </c>
       <c r="B110" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C110" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D110" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
@@ -2614,13 +2616,13 @@
         <v>2609402</v>
       </c>
       <c r="B111" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C111" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D111" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
@@ -2628,13 +2630,13 @@
         <v>2609501</v>
       </c>
       <c r="B112" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C112" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D112" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
@@ -2642,13 +2644,13 @@
         <v>2609600</v>
       </c>
       <c r="B113" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C113" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D113" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
@@ -2656,13 +2658,13 @@
         <v>2609709</v>
       </c>
       <c r="B114" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C114" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D114" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
@@ -2670,13 +2672,13 @@
         <v>2609808</v>
       </c>
       <c r="B115" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C115" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D115" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
@@ -2684,13 +2686,13 @@
         <v>2609907</v>
       </c>
       <c r="B116" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C116" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D116" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
@@ -2698,13 +2700,13 @@
         <v>2610004</v>
       </c>
       <c r="B117" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C117" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D117" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
@@ -2712,13 +2714,13 @@
         <v>2610103</v>
       </c>
       <c r="B118" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C118" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D118" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
@@ -2726,13 +2728,13 @@
         <v>2610202</v>
       </c>
       <c r="B119" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C119" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D119" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
@@ -2740,13 +2742,13 @@
         <v>2610301</v>
       </c>
       <c r="B120" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C120" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D120" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
@@ -2754,13 +2756,13 @@
         <v>2610400</v>
       </c>
       <c r="B121" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C121" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D121" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
@@ -2768,13 +2770,13 @@
         <v>2610509</v>
       </c>
       <c r="B122" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C122" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D122" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
@@ -2782,13 +2784,13 @@
         <v>2610608</v>
       </c>
       <c r="B123" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C123" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D123" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
@@ -2796,13 +2798,13 @@
         <v>2610707</v>
       </c>
       <c r="B124" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C124" t="s">
+        <v>4</v>
+      </c>
+      <c r="D124" t="s">
         <v>5</v>
-      </c>
-      <c r="D124" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
@@ -2810,13 +2812,13 @@
         <v>2610806</v>
       </c>
       <c r="B125" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C125" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D125" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
@@ -2824,13 +2826,13 @@
         <v>2610905</v>
       </c>
       <c r="B126" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C126" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D126" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
@@ -2838,13 +2840,13 @@
         <v>2611002</v>
       </c>
       <c r="B127" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C127" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D127" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
@@ -2852,13 +2854,13 @@
         <v>2611101</v>
       </c>
       <c r="B128" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C128" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D128" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
@@ -2866,13 +2868,13 @@
         <v>2611200</v>
       </c>
       <c r="B129" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C129" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D129" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
@@ -2880,13 +2882,13 @@
         <v>2611309</v>
       </c>
       <c r="B130" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C130" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D130" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.3">
@@ -2894,13 +2896,13 @@
         <v>2611408</v>
       </c>
       <c r="B131" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C131" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D131" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.3">
@@ -2908,13 +2910,13 @@
         <v>2611507</v>
       </c>
       <c r="B132" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C132" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D132" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.3">
@@ -2922,13 +2924,13 @@
         <v>2611533</v>
       </c>
       <c r="B133" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C133" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D133" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.3">
@@ -2936,13 +2938,13 @@
         <v>2611606</v>
       </c>
       <c r="B134" t="s">
+        <v>146</v>
+      </c>
+      <c r="C134" t="s">
         <v>147</v>
       </c>
-      <c r="C134" t="s">
-        <v>148</v>
-      </c>
       <c r="D134" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.3">
@@ -2950,13 +2952,13 @@
         <v>2611705</v>
       </c>
       <c r="B135" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C135" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D135" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.3">
@@ -2964,13 +2966,13 @@
         <v>2611804</v>
       </c>
       <c r="B136" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C136" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D136" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.3">
@@ -2978,13 +2980,13 @@
         <v>2611903</v>
       </c>
       <c r="B137" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C137" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D137" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.3">
@@ -2992,13 +2994,13 @@
         <v>2612000</v>
       </c>
       <c r="B138" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C138" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D138" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
@@ -3006,13 +3008,13 @@
         <v>2612109</v>
       </c>
       <c r="B139" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C139" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D139" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.3">
@@ -3020,13 +3022,13 @@
         <v>2612208</v>
       </c>
       <c r="B140" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C140" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D140" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.3">
@@ -3034,13 +3036,13 @@
         <v>2612307</v>
       </c>
       <c r="B141" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C141" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D141" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.3">
@@ -3048,13 +3050,13 @@
         <v>2612406</v>
       </c>
       <c r="B142" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C142" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D142" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.3">
@@ -3062,13 +3064,13 @@
         <v>2612455</v>
       </c>
       <c r="B143" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C143" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D143" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.3">
@@ -3076,13 +3078,13 @@
         <v>2612471</v>
       </c>
       <c r="B144" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C144" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D144" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.3">
@@ -3090,13 +3092,13 @@
         <v>2612505</v>
       </c>
       <c r="B145" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C145" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D145" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.3">
@@ -3104,13 +3106,13 @@
         <v>2612554</v>
       </c>
       <c r="B146" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C146" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D146" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
@@ -3118,13 +3120,13 @@
         <v>2612604</v>
       </c>
       <c r="B147" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C147" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D147" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
@@ -3132,13 +3134,13 @@
         <v>2612703</v>
       </c>
       <c r="B148" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C148" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D148" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
@@ -3146,13 +3148,13 @@
         <v>2612802</v>
       </c>
       <c r="B149" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C149" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D149" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
@@ -3160,13 +3162,13 @@
         <v>2612901</v>
       </c>
       <c r="B150" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C150" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D150" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
@@ -3174,13 +3176,13 @@
         <v>2613008</v>
       </c>
       <c r="B151" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C151" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D151" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.3">
@@ -3188,13 +3190,13 @@
         <v>2613107</v>
       </c>
       <c r="B152" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C152" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D152" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.3">
@@ -3202,13 +3204,13 @@
         <v>2613206</v>
       </c>
       <c r="B153" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C153" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D153" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.3">
@@ -3216,13 +3218,13 @@
         <v>2613305</v>
       </c>
       <c r="B154" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C154" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D154" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
@@ -3230,13 +3232,13 @@
         <v>2613404</v>
       </c>
       <c r="B155" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C155" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D155" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
@@ -3244,13 +3246,13 @@
         <v>2613503</v>
       </c>
       <c r="B156" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C156" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D156" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
@@ -3258,13 +3260,13 @@
         <v>2613602</v>
       </c>
       <c r="B157" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C157" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D157" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
@@ -3272,13 +3274,13 @@
         <v>2613701</v>
       </c>
       <c r="B158" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C158" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D158" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
@@ -3286,13 +3288,13 @@
         <v>2613800</v>
       </c>
       <c r="B159" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C159" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D159" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
@@ -3300,13 +3302,13 @@
         <v>2613909</v>
       </c>
       <c r="B160" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C160" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D160" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
@@ -3314,13 +3316,13 @@
         <v>2614006</v>
       </c>
       <c r="B161" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C161" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D161" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
@@ -3328,13 +3330,13 @@
         <v>2614105</v>
       </c>
       <c r="B162" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C162" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D162" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.3">
@@ -3342,13 +3344,13 @@
         <v>2614204</v>
       </c>
       <c r="B163" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C163" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D163" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.3">
@@ -3356,13 +3358,13 @@
         <v>2614402</v>
       </c>
       <c r="B164" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C164" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D164" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.3">
@@ -3370,13 +3372,13 @@
         <v>2614501</v>
       </c>
       <c r="B165" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C165" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D165" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
@@ -3384,13 +3386,13 @@
         <v>2614600</v>
       </c>
       <c r="B166" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C166" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D166" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
@@ -3398,13 +3400,13 @@
         <v>2614709</v>
       </c>
       <c r="B167" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C167" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D167" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
@@ -3412,13 +3414,13 @@
         <v>2614808</v>
       </c>
       <c r="B168" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C168" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D168" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
@@ -3426,13 +3428,13 @@
         <v>2614857</v>
       </c>
       <c r="B169" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C169" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D169" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
@@ -3440,13 +3442,13 @@
         <v>2615003</v>
       </c>
       <c r="B170" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C170" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D170" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
@@ -3454,13 +3456,13 @@
         <v>2615102</v>
       </c>
       <c r="B171" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C171" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D171" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
@@ -3468,13 +3470,13 @@
         <v>2615201</v>
       </c>
       <c r="B172" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C172" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D172" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
@@ -3482,13 +3484,13 @@
         <v>2615300</v>
       </c>
       <c r="B173" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C173" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D173" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.3">
@@ -3496,13 +3498,13 @@
         <v>2615409</v>
       </c>
       <c r="B174" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C174" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D174" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.3">
@@ -3510,13 +3512,13 @@
         <v>2615508</v>
       </c>
       <c r="B175" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C175" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D175" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.3">
@@ -3524,13 +3526,13 @@
         <v>2615607</v>
       </c>
       <c r="B176" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C176" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D176" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.3">
@@ -3538,13 +3540,13 @@
         <v>2615706</v>
       </c>
       <c r="B177" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C177" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D177" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.3">
@@ -3552,13 +3554,13 @@
         <v>2615805</v>
       </c>
       <c r="B178" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C178" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D178" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.3">
@@ -3566,13 +3568,13 @@
         <v>2615904</v>
       </c>
       <c r="B179" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C179" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D179" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.3">
@@ -3580,13 +3582,13 @@
         <v>2616001</v>
       </c>
       <c r="B180" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C180" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D180" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.3">
@@ -3594,13 +3596,13 @@
         <v>2616100</v>
       </c>
       <c r="B181" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C181" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D181" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
@@ -3608,13 +3610,13 @@
         <v>2616183</v>
       </c>
       <c r="B182" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C182" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D182" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.3">
@@ -3622,13 +3624,13 @@
         <v>2616209</v>
       </c>
       <c r="B183" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C183" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D183" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.3">
@@ -3636,13 +3638,13 @@
         <v>2616308</v>
       </c>
       <c r="B184" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C184" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D184" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
@@ -3650,13 +3652,13 @@
         <v>2616407</v>
       </c>
       <c r="B185" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C185" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D185" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.3">
@@ -3664,13 +3666,13 @@
         <v>2616506</v>
       </c>
       <c r="B186" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C186" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D186" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>